<commit_message>
added intial hazard validation to JAIS example
</commit_message>
<xml_diff>
--- a/examples/HEAT/JAIS_2023/topic_model_results/hazard_interpretation_SAFECOM_Final.xlsx
+++ b/examples/HEAT/JAIS_2023/topic_model_results/hazard_interpretation_SAFECOM_Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srandrad\smart_nlp\results\SAFECOM_hazards_lda_topics_Apr-04-2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srandrad\smart_nlp\examples\HEAT\JAIS_2023\topic_model_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F2646D-1B2C-49B0-AF91-4957D1DC054D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67917EB3-0679-461C-91D6-4A8FBA3D9684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="10044" firstSheet="1" activeTab="1" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="1" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hazard-focused" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="99">
   <si>
     <t>Hazard level 1 topics</t>
   </si>
@@ -91,9 +91,6 @@
     <t>topic 67 also discusses other fluid leaks</t>
   </si>
   <si>
-    <t>39, 7</t>
-  </si>
-  <si>
     <t>intrusion tfr, intruder, tfr, incursion, tfr intrusion, intrude tfr, tfr violation, tfr incursion, violate tfr, airspace conflict,  drone, enter tfr, drone sight, drone intrusion</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
     <t>0, 8, 30</t>
   </si>
   <si>
-    <t>jettison, jettison load, jettison retardant, jettison retardant load, load, retardant</t>
-  </si>
-  <si>
     <t>Tanker Loading Failure</t>
   </si>
   <si>
@@ -118,9 +112,6 @@
     <t>Radio Malfunction</t>
   </si>
   <si>
-    <t>5, 41, 85</t>
-  </si>
-  <si>
     <t>caution, master caution, light, master, illuminate, light illuminate, master caution panel, precautionary land, caution light illuminate, reset master, reset master caution, warn light, warn, warn light illuminate</t>
   </si>
   <si>
@@ -133,21 +124,12 @@
     <t>Inadequate PPE</t>
   </si>
   <si>
-    <t>11, 22</t>
-  </si>
-  <si>
     <t>circuit, breaker, circuit breaker, electrical, reset, switch, alternator, meter, popped, smell, panel, electrical power, wire, connection, loose, plug, wiring, loose wire, broken wire, cable</t>
   </si>
   <si>
     <t>Avionics Malfunction</t>
   </si>
   <si>
-    <t>13, 32, 92</t>
-  </si>
-  <si>
-    <t>wind, gust, condition, turbulence, inclement weather, inclement, climbed safe altitude, climbed safe, weather, visibility, fire behavior</t>
-  </si>
-  <si>
     <t>Severe Weather</t>
   </si>
   <si>
@@ -157,18 +139,9 @@
     <t>gear, retract, lock, main gear, nose, gear lock, gear retract, wheel, gear handle, left main gear, gear extend, nose wheel, land gear retract, right main gear, lock position, tire, flat</t>
   </si>
   <si>
-    <t>24, 25</t>
-  </si>
-  <si>
     <t>In-flight Collision</t>
   </si>
   <si>
-    <t>27, 37, 47</t>
-  </si>
-  <si>
-    <t>downwind, traffic, runway, traffic pattern, pattern, class airspace, airspace, tower, controller, airport, field, advisory, left downwind, restrict, airfield, announce, mid field, intention, vfr, turn downwind, enter traffic, flight restriction, temporary flight restriction, tfr, pattern, transponder, mapping, code, enter downwind, traffic advisory, restrict area, enter pattern, announce intention, aerial, observer, aerial observer, aerial detection, cautionary</t>
-  </si>
-  <si>
     <t>Airspace Control Hazards</t>
   </si>
   <si>
@@ -220,18 +193,9 @@
     <t>Intrusion</t>
   </si>
   <si>
-    <t>chip, chip light, light, transmission chip, plug, transmission, filter, chip plug, engine chip light, engine, recip engine, spark, spark plug, reciprocate, reciprocate engine, backfire, pop, compressor, bang, stall, compressor stall, gauge, power, normal, rpm, torque, generator, start, starter, battery, starter generator, white smoke come, white smoke, smoke</t>
-  </si>
-  <si>
-    <t>50, 54, 77, 82, 93, 64</t>
-  </si>
-  <si>
     <t>minor, sprain</t>
   </si>
   <si>
-    <t>duty, duty day, exceed, hour duty day</t>
-  </si>
-  <si>
     <t>hydraulic, hydraulic fluid, hydraulic pressure, hydraulic pump, hydraulic leak, hydraulic system, hydraulic fluid leak, hydraulic failure, fluid leak,  hydralic, loss hydraulic, hydraulics, notice hydraulic fluid, utility hydraulic, lose hydraulic pressure, hydrolic, hydraulic pump fail, hydraulic reservoir</t>
   </si>
   <si>
@@ -308,6 +272,66 @@
   </si>
   <si>
     <t>35, 41, 53, 55, 70, 67, 82, 30, 97, 14, 8, 80, 50, 76, 10, 44, 54, 71, 81, 84, 91, 96, 78, 23, 29, 32, 36, 38, 55, 83</t>
+  </si>
+  <si>
+    <t>Structural Damage</t>
+  </si>
+  <si>
+    <t>Communications Breakdown</t>
+  </si>
+  <si>
+    <t>chip, chip light, transmission chip, plug, transmission, filter, chip plug, engine chip light, engine, recip engine, spark, spark plug, reciprocate, reciprocate engine, backfire, pop, compressor, bang, stall, compressor stall, gauge, power, normal, rpm, torque, generator, start, starter, battery, starter generator, white smoke come, white smoke, smoke</t>
+  </si>
+  <si>
+    <t>inspection, crack, blade, rotor, tail, found, tail rotor, inch, damage, repair, shaft, cover, lead edge, broken, fuselage, tail rotor blade, rotor blade, hole, worn, approximately inch, main rotor blade, skin, small crack, dent, shear, loose, scratch, cowl, structural, wing, tear, pylon, possible, abnormality, defect, bent, airframe, flap, fin, delamination, inch crack</t>
+  </si>
+  <si>
+    <t>3, 24, 25</t>
+  </si>
+  <si>
+    <t>39, 7, 16</t>
+  </si>
+  <si>
+    <t>incorrect frequency, unable, issue, maintain positive communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jettison, jettison load, jettison retardant, jettison retardant load, load, retardant, aborted, abort, spill, overflow, malfunction, discharge </t>
+  </si>
+  <si>
+    <t>23, 35</t>
+  </si>
+  <si>
+    <t>wind, gust, condition, turbulence, inclement weather, inclement, climbed safe altitude, climbed safe, weather, visibility, fire behavior, fog, hazy, smoke</t>
+  </si>
+  <si>
+    <t>5, 41, 85, 53</t>
+  </si>
+  <si>
+    <t>68, 56</t>
+  </si>
+  <si>
+    <t>29, 72</t>
+  </si>
+  <si>
+    <t>duty, duty day, exceed, hour duty day,  past pumpkin time</t>
+  </si>
+  <si>
+    <t>12, 14, 28, 74</t>
+  </si>
+  <si>
+    <t>50, 54, 77, 82, 93, 64, 8, 41, 49, 83</t>
+  </si>
+  <si>
+    <t>11, 22, 83</t>
+  </si>
+  <si>
+    <t>13, 32, 92, 43, 87</t>
+  </si>
+  <si>
+    <t>downwind, traffic, runway, traffic pattern, pattern, class airspace, airspace, tower, controller, airport, field, advisory, left downwind, restrict, airfield, announce, mid field, intention, vfr, turn downwind, enter traffic, flight restriction, temporary flight restriction, tfr, pattern, transponder, mapping, code, enter downwind, traffic advisory, restrict area, enter pattern, announce intention, aerial, observer, aerial observer, aerial detection, cautionary, overflew, underflew, ifr, vfr</t>
+  </si>
+  <si>
+    <t>12, 27, 37, 47, 39, 69, 96</t>
   </si>
 </sst>
 </file>
@@ -718,10 +742,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E799D7D2-7755-4A40-8FAC-FBB6E32500C5}">
-  <dimension ref="A1:U27"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:S7"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -774,10 +798,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="N2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="R2" t="s">
         <v>14</v>
@@ -788,27 +812,27 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
       <c r="R3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>20</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
       </c>
       <c r="R4" t="s">
         <v>15</v>
@@ -816,30 +840,30 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>86</v>
+      </c>
+      <c r="R5" t="s">
         <v>22</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="R5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="R6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -850,27 +874,27 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="R7" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="U7" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="R8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -881,97 +905,97 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="R9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="R10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="N11" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="R11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="R12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="R13" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="R14" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>29</v>
+      <c r="A15" t="s">
+        <v>91</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="R15" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
@@ -982,69 +1006,69 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="R16" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="R17" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="R18" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="R19" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="N20" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="R20" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
@@ -1055,16 +1079,16 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="N21" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="R21" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="U21" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
@@ -1075,24 +1099,24 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="R22" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>68</v>
+      <c r="A23" t="s">
+        <v>90</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="R23" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
@@ -1103,10 +1127,10 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="R24" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
@@ -1117,30 +1141,30 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="N25" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="R25" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="N26" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="R26" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
@@ -1151,10 +1175,35 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="R27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>82</v>
+      </c>
+      <c r="R28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" t="s">
         <v>85</v>
+      </c>
+      <c r="R29" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>